<commit_message>
Optimizacion de rutas a sucursales
</commit_message>
<xml_diff>
--- a/data/dummy_data.xlsx
+++ b/data/dummy_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\PROJECTS\farmacia_alertas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C082A8F8-0B5F-4793-A7FC-E4168542E2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CF8482-1B6E-45BB-91E7-A5E01E7B235B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="proveedores" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4855" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4856" uniqueCount="823">
   <si>
     <t>proveedor_id</t>
   </si>
@@ -2525,7 +2525,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2548,20 +2548,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3138,19 +3148,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3161,7 +3171,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2">
         <v>1015</v>
       </c>
       <c r="B2" t="s">
@@ -3172,7 +3182,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>1024</v>
       </c>
       <c r="B3" t="s">
@@ -3183,7 +3193,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>1039</v>
       </c>
       <c r="B4" t="s">
@@ -3194,7 +3204,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>1040</v>
       </c>
       <c r="B5" t="s">
@@ -3205,7 +3215,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>1065</v>
       </c>
       <c r="B6" t="s">
@@ -3216,7 +3226,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>1067</v>
       </c>
       <c r="B7" t="s">
@@ -3227,7 +3237,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>1068</v>
       </c>
       <c r="B8" t="s">
@@ -3238,7 +3248,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>1071</v>
       </c>
       <c r="B9" t="s">
@@ -3249,7 +3259,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>1073</v>
       </c>
       <c r="B10" t="s">
@@ -3260,7 +3270,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>1076</v>
       </c>
       <c r="B11" t="s">
@@ -3271,7 +3281,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>1087</v>
       </c>
       <c r="B12" t="s">
@@ -3282,7 +3292,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>1089</v>
       </c>
       <c r="B13" t="s">
@@ -3293,7 +3303,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>1099</v>
       </c>
       <c r="B14" t="s">
@@ -3304,7 +3314,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>1111</v>
       </c>
       <c r="B15" t="s">
@@ -3315,7 +3325,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>1151</v>
       </c>
       <c r="B16" t="s">
@@ -3326,7 +3336,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17">
         <v>1158</v>
       </c>
       <c r="B17" t="s">
@@ -3337,7 +3347,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18">
         <v>1172</v>
       </c>
       <c r="B18" t="s">
@@ -3348,7 +3358,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19">
         <v>1174</v>
       </c>
       <c r="B19" t="s">
@@ -3359,7 +3369,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20">
         <v>1184</v>
       </c>
       <c r="B20" t="s">
@@ -3370,7 +3380,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21">
         <v>1220</v>
       </c>
       <c r="B21" t="s">
@@ -3381,7 +3391,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22">
         <v>1242</v>
       </c>
       <c r="B22" t="s">
@@ -3392,7 +3402,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23">
         <v>1250</v>
       </c>
       <c r="B23" t="s">
@@ -3403,7 +3413,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24">
         <v>1255</v>
       </c>
       <c r="B24" t="s">
@@ -3414,7 +3424,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25">
         <v>1279</v>
       </c>
       <c r="B25" t="s">
@@ -3425,7 +3435,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26">
         <v>1280</v>
       </c>
       <c r="B26" t="s">
@@ -3436,7 +3446,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27">
         <v>1284</v>
       </c>
       <c r="B27" t="s">
@@ -3447,7 +3457,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28">
         <v>1285</v>
       </c>
       <c r="B28" t="s">
@@ -3458,7 +3468,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29">
         <v>1292</v>
       </c>
       <c r="B29" t="s">
@@ -3469,7 +3479,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30">
         <v>1301</v>
       </c>
       <c r="B30" t="s">
@@ -3480,7 +3490,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31">
         <v>1329</v>
       </c>
       <c r="B31" t="s">
@@ -3491,7 +3501,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32">
         <v>1342</v>
       </c>
       <c r="B32" t="s">
@@ -3502,7 +3512,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33">
         <v>1343</v>
       </c>
       <c r="B33" t="s">
@@ -3513,7 +3523,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34">
         <v>1355</v>
       </c>
       <c r="B34" t="s">
@@ -3524,7 +3534,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35">
         <v>1374</v>
       </c>
       <c r="B35" t="s">
@@ -3535,7 +3545,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36">
         <v>1378</v>
       </c>
       <c r="B36" t="s">
@@ -3546,7 +3556,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37">
         <v>1418</v>
       </c>
       <c r="B37" t="s">
@@ -3557,7 +3567,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38">
         <v>1421</v>
       </c>
       <c r="B38" t="s">
@@ -3568,7 +3578,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39">
         <v>1422</v>
       </c>
       <c r="B39" t="s">
@@ -3579,7 +3589,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40">
         <v>1460</v>
       </c>
       <c r="B40" t="s">
@@ -3590,7 +3600,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41">
         <v>1462</v>
       </c>
       <c r="B41" t="s">
@@ -3601,7 +3611,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42">
         <v>1492</v>
       </c>
       <c r="B42" t="s">
@@ -3612,7 +3622,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43">
         <v>1508</v>
       </c>
       <c r="B43" t="s">
@@ -3623,7 +3633,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44">
         <v>1509</v>
       </c>
       <c r="B44" t="s">
@@ -3634,7 +3644,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45">
         <v>1514</v>
       </c>
       <c r="B45" t="s">
@@ -3645,7 +3655,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46">
         <v>1517</v>
       </c>
       <c r="B46" t="s">
@@ -3656,7 +3666,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47">
         <v>1536</v>
       </c>
       <c r="B47" t="s">
@@ -3667,7 +3677,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48">
         <v>1556</v>
       </c>
       <c r="B48" t="s">
@@ -3678,7 +3688,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="A49">
         <v>1557</v>
       </c>
       <c r="B49" t="s">
@@ -3689,7 +3699,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50">
         <v>1558</v>
       </c>
       <c r="B50" t="s">
@@ -3700,7 +3710,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51">
         <v>1559</v>
       </c>
       <c r="B51" t="s">
@@ -3711,7 +3721,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52">
         <v>1577</v>
       </c>
       <c r="B52" t="s">
@@ -3722,7 +3732,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53">
         <v>1588</v>
       </c>
       <c r="B53" t="s">
@@ -3733,7 +3743,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="A54">
         <v>1591</v>
       </c>
       <c r="B54" t="s">
@@ -3744,7 +3754,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="A55">
         <v>1592</v>
       </c>
       <c r="B55" t="s">
@@ -3755,7 +3765,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="A56">
         <v>1594</v>
       </c>
       <c r="B56" t="s">
@@ -3766,7 +3776,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57">
         <v>1597</v>
       </c>
       <c r="B57" t="s">
@@ -3777,7 +3787,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="A58">
         <v>1598</v>
       </c>
       <c r="B58" t="s">
@@ -3788,7 +3798,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="A59">
         <v>1600</v>
       </c>
       <c r="B59" t="s">
@@ -3799,7 +3809,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="A60">
         <v>1601</v>
       </c>
       <c r="B60" t="s">
@@ -3810,7 +3820,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="A61">
         <v>1605</v>
       </c>
       <c r="B61" t="s">
@@ -3821,7 +3831,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="A62">
         <v>1610</v>
       </c>
       <c r="B62" t="s">
@@ -3832,7 +3842,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="A63">
         <v>1627</v>
       </c>
       <c r="B63" t="s">
@@ -3843,7 +3853,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="A64">
         <v>1649</v>
       </c>
       <c r="B64" t="s">
@@ -3854,7 +3864,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="A65">
         <v>1655</v>
       </c>
       <c r="B65" t="s">
@@ -3865,7 +3875,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="A66">
         <v>1658</v>
       </c>
       <c r="B66" t="s">
@@ -3876,7 +3886,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="A67">
         <v>1704</v>
       </c>
       <c r="B67" t="s">
@@ -3887,7 +3897,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="A68">
         <v>1705</v>
       </c>
       <c r="B68" t="s">
@@ -3898,7 +3908,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="A69">
         <v>1908</v>
       </c>
       <c r="B69" t="s">
@@ -3909,7 +3919,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70">
         <v>1999</v>
       </c>
       <c r="B70" t="s">
@@ -3920,7 +3930,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="A71">
         <v>2054</v>
       </c>
       <c r="B71" t="s">
@@ -3931,7 +3941,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="A72">
         <v>2077</v>
       </c>
       <c r="B72" t="s">
@@ -3942,7 +3952,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="A73">
         <v>2078</v>
       </c>
       <c r="B73" t="s">
@@ -3953,7 +3963,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="A74">
         <v>2082</v>
       </c>
       <c r="B74" t="s">
@@ -3964,7 +3974,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="A75">
         <v>2088</v>
       </c>
       <c r="B75" t="s">
@@ -3975,7 +3985,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="A76">
         <v>2089</v>
       </c>
       <c r="B76" t="s">
@@ -3986,7 +3996,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="A77">
         <v>2120</v>
       </c>
       <c r="B77" t="s">
@@ -3997,7 +4007,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="A78">
         <v>2146</v>
       </c>
       <c r="B78" t="s">
@@ -4008,7 +4018,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="A79">
         <v>2151</v>
       </c>
       <c r="B79" t="s">
@@ -4019,7 +4029,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="A80">
         <v>2167</v>
       </c>
       <c r="B80" t="s">
@@ -4030,7 +4040,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="A81">
         <v>2168</v>
       </c>
       <c r="B81" t="s">
@@ -4041,7 +4051,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="A82">
         <v>2202</v>
       </c>
       <c r="B82" t="s">
@@ -4052,7 +4062,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="A83">
         <v>2212</v>
       </c>
       <c r="B83" t="s">
@@ -4063,7 +4073,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="A84">
         <v>10631</v>
       </c>
       <c r="B84" t="s">
@@ -4074,7 +4084,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="A85">
         <v>11565</v>
       </c>
       <c r="B85" t="s">
@@ -4085,7 +4095,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="A86">
         <v>11585</v>
       </c>
       <c r="B86" t="s">
@@ -4096,7 +4106,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="A87">
         <v>300651429312</v>
       </c>
       <c r="B87" t="s">
@@ -4107,7 +4117,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+      <c r="A88">
         <v>300651431681</v>
       </c>
       <c r="B88" t="s">
@@ -4118,7 +4128,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="A89">
         <v>736085011937</v>
       </c>
       <c r="B89" t="s">
@@ -4129,7 +4139,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="A90">
         <v>736085401431</v>
       </c>
       <c r="B90" t="s">
@@ -4140,7 +4150,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="A91">
         <v>736085402346</v>
       </c>
       <c r="B91" t="s">
@@ -4151,7 +4161,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="A92">
         <v>736085412734</v>
       </c>
       <c r="B92" t="s">
@@ -4162,7 +4172,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="A93">
         <v>736085416909</v>
       </c>
       <c r="B93" t="s">
@@ -4173,7 +4183,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+      <c r="A94">
         <v>736085905373</v>
       </c>
       <c r="B94" t="s">
@@ -4184,7 +4194,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+      <c r="A95">
         <v>3594454400846</v>
       </c>
       <c r="B95" t="s">
@@ -4195,7 +4205,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
+      <c r="A96">
         <v>3594455200162</v>
       </c>
       <c r="B96" t="s">
@@ -4206,7 +4216,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
+      <c r="A97">
         <v>3594455600153</v>
       </c>
       <c r="B97" t="s">
@@ -4217,7 +4227,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+      <c r="A98">
         <v>3664898060675</v>
       </c>
       <c r="B98" t="s">
@@ -4228,7 +4238,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+      <c r="A99">
         <v>4008491317061</v>
       </c>
       <c r="B99" t="s">
@@ -4239,7 +4249,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+      <c r="A100">
         <v>4260095689368</v>
       </c>
       <c r="B100" t="s">
@@ -4250,7 +4260,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+      <c r="A101">
         <v>4260095689375</v>
       </c>
       <c r="B101" t="s">
@@ -4261,7 +4271,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="A102">
         <v>5000456033381</v>
       </c>
       <c r="B102" t="s">
@@ -4272,7 +4282,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+      <c r="A103">
         <v>5000456076692</v>
       </c>
       <c r="B103" t="s">
@@ -4283,7 +4293,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+      <c r="A104">
         <v>5000456076715</v>
       </c>
       <c r="B104" t="s">
@@ -4294,7 +4304,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
+      <c r="A105">
         <v>5056227208274</v>
       </c>
       <c r="B105" t="s">
@@ -4305,7 +4315,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
+      <c r="A106">
         <v>5391189310673</v>
       </c>
       <c r="B106" t="s">
@@ -4316,7 +4326,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
+      <c r="A107">
         <v>5391189330671</v>
       </c>
       <c r="B107" t="s">
@@ -4327,7 +4337,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+      <c r="A108">
         <v>7501033921759</v>
       </c>
       <c r="B108" t="s">
@@ -4338,7 +4348,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="4">
+      <c r="A109">
         <v>7501033923173</v>
       </c>
       <c r="B109" t="s">
@@ -4349,7 +4359,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
+      <c r="A110">
         <v>7501033923241</v>
       </c>
       <c r="B110" t="s">
@@ -4360,7 +4370,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
+      <c r="A111">
         <v>7501033953057</v>
       </c>
       <c r="B111" t="s">
@@ -4371,7 +4381,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
+      <c r="A112">
         <v>7501033957871</v>
       </c>
       <c r="B112" t="s">
@@ -4382,7 +4392,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4">
+      <c r="A113">
         <v>7501033959912</v>
       </c>
       <c r="B113" t="s">
@@ -4393,7 +4403,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="4">
+      <c r="A114">
         <v>7501033960543</v>
       </c>
       <c r="B114" t="s">
@@ -4404,7 +4414,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="4">
+      <c r="A115">
         <v>7501034600196</v>
       </c>
       <c r="B115" t="s">
@@ -4415,7 +4425,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+      <c r="A116">
         <v>7501034630131</v>
       </c>
       <c r="B116" t="s">
@@ -4426,7 +4436,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
+      <c r="A117">
         <v>7501034664082</v>
       </c>
       <c r="B117" t="s">
@@ -4437,7 +4447,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
+      <c r="A118">
         <v>7501034692184</v>
       </c>
       <c r="B118" t="s">
@@ -4448,7 +4458,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
+      <c r="A119">
         <v>7501037920147</v>
       </c>
       <c r="B119" t="s">
@@ -4459,7 +4469,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
+      <c r="A120">
         <v>7501037935189</v>
       </c>
       <c r="B120" t="s">
@@ -4470,7 +4480,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="4">
+      <c r="A121">
         <v>7501043101011</v>
       </c>
       <c r="B121" t="s">
@@ -4481,7 +4491,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
+      <c r="A122">
         <v>7501043166522</v>
       </c>
       <c r="B122" t="s">
@@ -4492,7 +4502,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
+      <c r="A123">
         <v>7501050617611</v>
       </c>
       <c r="B123" t="s">
@@ -4503,7 +4513,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4">
+      <c r="A124">
         <v>7501050632034</v>
       </c>
       <c r="B124" t="s">
@@ -4514,7 +4524,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="4">
+      <c r="A125">
         <v>7501070615451</v>
       </c>
       <c r="B125" t="s">
@@ -4525,7 +4535,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
+      <c r="A126">
         <v>7501070648022</v>
       </c>
       <c r="B126" t="s">
@@ -4536,7 +4546,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="4">
+      <c r="A127">
         <v>7501070903459</v>
       </c>
       <c r="B127" t="s">
@@ -4547,7 +4557,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
+      <c r="A128">
         <v>7501082208764</v>
       </c>
       <c r="B128" t="s">
@@ -4558,7 +4568,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="4">
+      <c r="A129">
         <v>7501082242096</v>
       </c>
       <c r="B129" t="s">
@@ -4569,7 +4579,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+      <c r="A130">
         <v>7501088507007</v>
       </c>
       <c r="B130" t="s">
@@ -4580,7 +4590,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
+      <c r="A131">
         <v>7501088507601</v>
       </c>
       <c r="B131" t="s">
@@ -4591,7 +4601,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
+      <c r="A132">
         <v>7501088507694</v>
       </c>
       <c r="B132" t="s">
@@ -4602,7 +4612,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
+      <c r="A133">
         <v>7501088531002</v>
       </c>
       <c r="B133" t="s">
@@ -4613,7 +4623,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
+      <c r="A134">
         <v>7501089801098</v>
       </c>
       <c r="B134" t="s">
@@ -4624,7 +4634,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
+      <c r="A135">
         <v>7501089802019</v>
       </c>
       <c r="B135" t="s">
@@ -4635,7 +4645,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+      <c r="A136">
         <v>7501089802071</v>
       </c>
       <c r="B136" t="s">
@@ -4646,7 +4656,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="4">
+      <c r="A137">
         <v>7501089802453</v>
       </c>
       <c r="B137" t="s">
@@ -4657,7 +4667,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+      <c r="A138">
         <v>7501089803054</v>
       </c>
       <c r="B138" t="s">
@@ -4668,7 +4678,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
+      <c r="A139">
         <v>7501089803160</v>
       </c>
       <c r="B139" t="s">
@@ -4679,7 +4689,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="4">
+      <c r="A140">
         <v>7501089803177</v>
       </c>
       <c r="B140" t="s">
@@ -4690,7 +4700,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
+      <c r="A141">
         <v>7501089830180</v>
       </c>
       <c r="B141" t="s">
@@ -4701,7 +4711,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="4">
+      <c r="A142">
         <v>7501094916640</v>
       </c>
       <c r="B142" t="s">
@@ -4712,7 +4722,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="4">
+      <c r="A143">
         <v>7501094916671</v>
       </c>
       <c r="B143" t="s">
@@ -4723,7 +4733,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="4">
+      <c r="A144">
         <v>7501094916794</v>
       </c>
       <c r="B144" t="s">
@@ -4734,7 +4744,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="4">
+      <c r="A145">
         <v>7501094917005</v>
       </c>
       <c r="B145" t="s">
@@ -4745,7 +4755,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="4">
+      <c r="A146">
         <v>7501094917012</v>
       </c>
       <c r="B146" t="s">
@@ -4756,7 +4766,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="4">
+      <c r="A147">
         <v>7501094917029</v>
       </c>
       <c r="B147" t="s">
@@ -4767,7 +4777,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="4">
+      <c r="A148">
         <v>7501098604499</v>
       </c>
       <c r="B148" t="s">
@@ -4778,7 +4788,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="4">
+      <c r="A149">
         <v>7501098604505</v>
       </c>
       <c r="B149" t="s">
@@ -4789,7 +4799,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="4">
+      <c r="A150">
         <v>7501098604529</v>
       </c>
       <c r="B150" t="s">
@@ -4800,7 +4810,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="4">
+      <c r="A151">
         <v>7501098610025</v>
       </c>
       <c r="B151" t="s">
@@ -4811,7 +4821,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="4">
+      <c r="A152">
         <v>7501098610032</v>
       </c>
       <c r="B152" t="s">
@@ -4822,7 +4832,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="4">
+      <c r="A153">
         <v>7501098610810</v>
       </c>
       <c r="B153" t="s">
@@ -4833,7 +4843,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="4">
+      <c r="A154">
         <v>7501098633260</v>
       </c>
       <c r="B154" t="s">
@@ -4844,7 +4854,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="4">
+      <c r="A155">
         <v>7501101600630</v>
       </c>
       <c r="B155" t="s">
@@ -4855,7 +4865,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="4">
+      <c r="A156">
         <v>7501101602078</v>
       </c>
       <c r="B156" t="s">
@@ -4866,7 +4876,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="4">
+      <c r="A157">
         <v>7501101602108</v>
       </c>
       <c r="B157" t="s">
@@ -4877,7 +4887,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="4">
+      <c r="A158">
         <v>7501101611018</v>
       </c>
       <c r="B158" t="s">
@@ -4888,7 +4898,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="4">
+      <c r="A159">
         <v>7501101611162</v>
       </c>
       <c r="B159" t="s">
@@ -4899,7 +4909,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="4">
+      <c r="A160">
         <v>7501101611544</v>
       </c>
       <c r="B160" t="s">
@@ -4910,7 +4920,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="4">
+      <c r="A161">
         <v>7501101611568</v>
       </c>
       <c r="B161" t="s">
@@ -4921,7 +4931,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="4">
+      <c r="A162">
         <v>7501101615016</v>
       </c>
       <c r="B162" t="s">
@@ -4932,7 +4942,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="4">
+      <c r="A163">
         <v>7501101623349</v>
       </c>
       <c r="B163" t="s">
@@ -4943,7 +4953,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="4">
+      <c r="A164">
         <v>7501101643217</v>
       </c>
       <c r="B164" t="s">
@@ -4954,7 +4964,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="4">
+      <c r="A165">
         <v>7501108712138</v>
       </c>
       <c r="B165" t="s">
@@ -4965,7 +4975,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="4">
+      <c r="A166">
         <v>7501109901517</v>
       </c>
       <c r="B166" t="s">
@@ -4976,7 +4986,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="4">
+      <c r="A167">
         <v>7501109930135</v>
       </c>
       <c r="B167" t="s">
@@ -4987,7 +4997,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="4">
+      <c r="A168">
         <v>7501124183493</v>
       </c>
       <c r="B168" t="s">
@@ -4998,7 +5008,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="4">
+      <c r="A169">
         <v>7501124815899</v>
       </c>
       <c r="B169" t="s">
@@ -5009,7 +5019,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="4">
+      <c r="A170">
         <v>7501124819293</v>
       </c>
       <c r="B170" t="s">
@@ -5020,7 +5030,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="4">
+      <c r="A171">
         <v>7501124819385</v>
       </c>
       <c r="B171" t="s">
@@ -5031,7 +5041,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="4">
+      <c r="A172">
         <v>7501124820312</v>
       </c>
       <c r="B172" t="s">
@@ -5042,7 +5052,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="4">
+      <c r="A173">
         <v>7501124820558</v>
       </c>
       <c r="B173" t="s">
@@ -5053,7 +5063,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="4">
+      <c r="A174">
         <v>7501124820664</v>
       </c>
       <c r="B174" t="s">
@@ -5064,7 +5074,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="4">
+      <c r="A175">
         <v>7501124820817</v>
       </c>
       <c r="B175" t="s">
@@ -5075,7 +5085,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="4">
+      <c r="A176">
         <v>7501125114717</v>
       </c>
       <c r="B176" t="s">
@@ -5086,7 +5096,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="4">
+      <c r="A177">
         <v>7501125154621</v>
       </c>
       <c r="B177" t="s">
@@ -5097,7 +5107,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="4">
+      <c r="A178">
         <v>7501125159329</v>
       </c>
       <c r="B178" t="s">
@@ -5108,7 +5118,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="4">
+      <c r="A179">
         <v>7501125159633</v>
       </c>
       <c r="B179" t="s">
@@ -5119,7 +5129,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="4">
+      <c r="A180">
         <v>7501125161278</v>
       </c>
       <c r="B180" t="s">
@@ -5130,7 +5140,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="4">
+      <c r="A181">
         <v>7501125162817</v>
       </c>
       <c r="B181" t="s">
@@ -5141,7 +5151,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="4">
+      <c r="A182">
         <v>7501125164668</v>
       </c>
       <c r="B182" t="s">
@@ -5152,7 +5162,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="4">
+      <c r="A183">
         <v>7501125165276</v>
       </c>
       <c r="B183" t="s">
@@ -5163,7 +5173,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="4">
+      <c r="A184">
         <v>7501125165665</v>
       </c>
       <c r="B184" t="s">
@@ -5174,7 +5184,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="4">
+      <c r="A185">
         <v>7501165000193</v>
       </c>
       <c r="B185" t="s">
@@ -5185,7 +5195,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="4">
+      <c r="A186">
         <v>7501165007192</v>
       </c>
       <c r="B186" t="s">
@@ -5196,7 +5206,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="4">
+      <c r="A187">
         <v>7501165007796</v>
       </c>
       <c r="B187" t="s">
@@ -5207,7 +5217,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="4">
+      <c r="A188">
         <v>7501165007833</v>
       </c>
       <c r="B188" t="s">
@@ -5218,7 +5228,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="4">
+      <c r="A189">
         <v>7501165010635</v>
       </c>
       <c r="B189" t="s">
@@ -5229,7 +5239,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="4">
+      <c r="A190">
         <v>7501168870625</v>
       </c>
       <c r="B190" t="s">
@@ -5240,7 +5250,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="4">
+      <c r="A191">
         <v>7501201400833</v>
       </c>
       <c r="B191" t="s">
@@ -5251,7 +5261,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="4">
+      <c r="A192">
         <v>7501249600820</v>
       </c>
       <c r="B192" t="s">
@@ -5262,7 +5272,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="4">
+      <c r="A193">
         <v>7501249601322</v>
       </c>
       <c r="B193" t="s">
@@ -5273,7 +5283,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="4">
+      <c r="A194">
         <v>7501249605252</v>
       </c>
       <c r="B194" t="s">
@@ -5284,7 +5294,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="4">
+      <c r="A195">
         <v>7501249605405</v>
       </c>
       <c r="B195" t="s">
@@ -5295,7 +5305,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="4">
+      <c r="A196">
         <v>7501249605412</v>
       </c>
       <c r="B196" t="s">
@@ -5306,7 +5316,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="4">
+      <c r="A197">
         <v>7501249605429</v>
       </c>
       <c r="B197" t="s">
@@ -5317,7 +5327,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="4">
+      <c r="A198">
         <v>7501249605436</v>
       </c>
       <c r="B198" t="s">
@@ -5328,7 +5338,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="4">
+      <c r="A199">
         <v>7501249605788</v>
       </c>
       <c r="B199" t="s">
@@ -5339,7 +5349,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="4">
+      <c r="A200">
         <v>7501249605801</v>
       </c>
       <c r="B200" t="s">
@@ -5350,7 +5360,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="4">
+      <c r="A201">
         <v>7501249605818</v>
       </c>
       <c r="B201" t="s">
@@ -5361,7 +5371,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="4">
+      <c r="A202">
         <v>7501249605849</v>
       </c>
       <c r="B202" t="s">
@@ -5372,7 +5382,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="4">
+      <c r="A203">
         <v>7501249607898</v>
       </c>
       <c r="B203" t="s">
@@ -5383,7 +5393,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="4">
+      <c r="A204">
         <v>7501249608055</v>
       </c>
       <c r="B204" t="s">
@@ -5394,7 +5404,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="4">
+      <c r="A205">
         <v>7501250838946</v>
       </c>
       <c r="B205" t="s">
@@ -5405,7 +5415,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="4">
+      <c r="A206">
         <v>7501285600075</v>
       </c>
       <c r="B206" t="s">
@@ -5416,7 +5426,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="4">
+      <c r="A207">
         <v>7501287670038</v>
       </c>
       <c r="B207" t="s">
@@ -5427,7 +5437,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="4">
+      <c r="A208">
         <v>7501298204987</v>
       </c>
       <c r="B208" t="s">
@@ -5438,7 +5448,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="4">
+      <c r="A209">
         <v>7501298205038</v>
       </c>
       <c r="B209" t="s">
@@ -5449,7 +5459,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="4">
+      <c r="A210">
         <v>7501298206455</v>
       </c>
       <c r="B210" t="s">
@@ -5460,7 +5470,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="4">
+      <c r="A211">
         <v>7501298213040</v>
       </c>
       <c r="B211" t="s">
@@ -5471,7 +5481,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="4">
+      <c r="A212">
         <v>7501298214207</v>
       </c>
       <c r="B212" t="s">
@@ -5482,7 +5492,7 @@
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="4">
+      <c r="A213">
         <v>7501298216812</v>
       </c>
       <c r="B213" t="s">
@@ -5493,7 +5503,7 @@
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="4">
+      <c r="A214">
         <v>7501298217130</v>
       </c>
       <c r="B214" t="s">
@@ -5504,7 +5514,7 @@
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="4">
+      <c r="A215">
         <v>7501298219608</v>
       </c>
       <c r="B215" t="s">
@@ -5515,7 +5525,7 @@
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="4">
+      <c r="A216">
         <v>7501298222424</v>
       </c>
       <c r="B216" t="s">
@@ -5526,7 +5536,7 @@
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="4">
+      <c r="A217">
         <v>7501298222509</v>
       </c>
       <c r="B217" t="s">
@@ -5537,7 +5547,7 @@
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="4">
+      <c r="A218">
         <v>7501298234601</v>
       </c>
       <c r="B218" t="s">
@@ -5548,7 +5558,7 @@
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="4">
+      <c r="A219">
         <v>7501298234700</v>
       </c>
       <c r="B219" t="s">
@@ -5559,7 +5569,7 @@
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="4">
+      <c r="A220">
         <v>7501298234809</v>
       </c>
       <c r="B220" t="s">
@@ -5570,7 +5580,7 @@
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="4">
+      <c r="A221">
         <v>7501298234908</v>
       </c>
       <c r="B221" t="s">
@@ -5581,7 +5591,7 @@
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="4">
+      <c r="A222">
         <v>7501298244907</v>
       </c>
       <c r="B222" t="s">
@@ -5592,7 +5602,7 @@
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="4">
+      <c r="A223">
         <v>7501298269009</v>
       </c>
       <c r="B223" t="s">
@@ -5603,7 +5613,7 @@
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="4">
+      <c r="A224">
         <v>7501299307144</v>
       </c>
       <c r="B224" t="s">
@@ -5614,7 +5624,7 @@
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="4">
+      <c r="A225">
         <v>7501299307526</v>
       </c>
       <c r="B225" t="s">
@@ -5625,7 +5635,7 @@
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="4">
+      <c r="A226">
         <v>7501299308806</v>
       </c>
       <c r="B226" t="s">
@@ -5636,7 +5646,7 @@
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="4">
+      <c r="A227">
         <v>7501300406651</v>
       </c>
       <c r="B227" t="s">
@@ -5647,7 +5657,7 @@
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="4">
+      <c r="A228">
         <v>7501300407962</v>
       </c>
       <c r="B228" t="s">
@@ -5658,7 +5668,7 @@
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="4">
+      <c r="A229">
         <v>7501300408174</v>
       </c>
       <c r="B229" t="s">
@@ -5669,7 +5679,7 @@
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="4">
+      <c r="A230">
         <v>7501300408730</v>
       </c>
       <c r="B230" t="s">
@@ -5680,7 +5690,7 @@
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="4">
+      <c r="A231">
         <v>7501300420091</v>
       </c>
       <c r="B231" t="s">
@@ -5691,7 +5701,7 @@
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="4">
+      <c r="A232">
         <v>7501300420374</v>
       </c>
       <c r="B232" t="s">
@@ -5702,7 +5712,7 @@
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="4">
+      <c r="A233">
         <v>7501300420398</v>
       </c>
       <c r="B233" t="s">
@@ -5713,7 +5723,7 @@
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="4">
+      <c r="A234">
         <v>7501300420626</v>
       </c>
       <c r="B234" t="s">
@@ -5724,7 +5734,7 @@
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="4">
+      <c r="A235">
         <v>7501300420640</v>
       </c>
       <c r="B235" t="s">
@@ -5735,7 +5745,7 @@
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="4">
+      <c r="A236">
         <v>7501303442601</v>
       </c>
       <c r="B236" t="s">
@@ -5746,7 +5756,7 @@
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="4">
+      <c r="A237">
         <v>7501303444001</v>
       </c>
       <c r="B237" t="s">
@@ -5757,7 +5767,7 @@
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="4">
+      <c r="A238">
         <v>7501303451603</v>
       </c>
       <c r="B238" t="s">
@@ -5768,7 +5778,7 @@
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="4">
+      <c r="A239">
         <v>7501303457513</v>
       </c>
       <c r="B239" t="s">
@@ -5779,7 +5789,7 @@
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="4">
+      <c r="A240">
         <v>7501314705535</v>
       </c>
       <c r="B240" t="s">
@@ -5790,7 +5800,7 @@
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="4">
+      <c r="A241">
         <v>7501318608788</v>
       </c>
       <c r="B241" t="s">
@@ -5801,7 +5811,7 @@
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="4">
+      <c r="A242">
         <v>7501318612082</v>
       </c>
       <c r="B242" t="s">
@@ -5812,7 +5822,7 @@
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="4">
+      <c r="A243">
         <v>7501318612655</v>
       </c>
       <c r="B243" t="s">
@@ -5823,7 +5833,7 @@
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="4">
+      <c r="A244">
         <v>7501318673205</v>
       </c>
       <c r="B244" t="s">
@@ -5834,7 +5844,7 @@
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="4">
+      <c r="A245">
         <v>7501318681422</v>
       </c>
       <c r="B245" t="s">
@@ -5845,7 +5855,7 @@
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="4">
+      <c r="A246">
         <v>7501326001137</v>
       </c>
       <c r="B246" t="s">
@@ -5856,7 +5866,7 @@
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="4">
+      <c r="A247">
         <v>7501326004176</v>
       </c>
       <c r="B247" t="s">
@@ -5867,7 +5877,7 @@
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" s="4">
+      <c r="A248">
         <v>7501326004947</v>
       </c>
       <c r="B248" t="s">
@@ -5878,7 +5888,7 @@
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" s="4">
+      <c r="A249">
         <v>7501326008402</v>
       </c>
       <c r="B249" t="s">
@@ -5889,7 +5899,7 @@
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" s="4">
+      <c r="A250">
         <v>7501328977980</v>
       </c>
       <c r="B250" t="s">
@@ -5900,7 +5910,7 @@
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="4">
+      <c r="A251">
         <v>7501328979564</v>
       </c>
       <c r="B251" t="s">
@@ -5911,7 +5921,7 @@
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="4">
+      <c r="A252">
         <v>7501328979601</v>
       </c>
       <c r="B252" t="s">
@@ -5922,7 +5932,7 @@
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="4">
+      <c r="A253">
         <v>7501328980034</v>
       </c>
       <c r="B253" t="s">
@@ -5933,7 +5943,7 @@
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="4">
+      <c r="A254">
         <v>7501349021327</v>
       </c>
       <c r="B254" t="s">
@@ -5944,7 +5954,7 @@
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" s="4">
+      <c r="A255">
         <v>7501361693045</v>
       </c>
       <c r="B255" t="s">
@@ -5955,7 +5965,7 @@
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256" s="4">
+      <c r="A256">
         <v>7501384502331</v>
       </c>
       <c r="B256" t="s">
@@ -5966,7 +5976,7 @@
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="4">
+      <c r="A257">
         <v>7501384503307</v>
       </c>
       <c r="B257" t="s">
@@ -5977,7 +5987,7 @@
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="4">
+      <c r="A258">
         <v>7501384545352</v>
       </c>
       <c r="B258" t="s">
@@ -5988,7 +5998,7 @@
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="4">
+      <c r="A259">
         <v>7501385420221</v>
       </c>
       <c r="B259" t="s">
@@ -5999,7 +6009,7 @@
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="4">
+      <c r="A260">
         <v>7501409201102</v>
       </c>
       <c r="B260" t="s">
@@ -6010,7 +6020,7 @@
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="4">
+      <c r="A261">
         <v>7501409201522</v>
       </c>
       <c r="B261" t="s">
@@ -6021,7 +6031,7 @@
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="4">
+      <c r="A262">
         <v>7501559612506</v>
       </c>
       <c r="B262" t="s">
@@ -6032,7 +6042,7 @@
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="4">
+      <c r="A263">
         <v>7501701408735</v>
       </c>
       <c r="B263" t="s">
@@ -6043,7 +6053,7 @@
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="4">
+      <c r="A264">
         <v>7501871720880</v>
       </c>
       <c r="B264" t="s">
@@ -6054,7 +6064,7 @@
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265" s="4">
+      <c r="A265">
         <v>7501871720941</v>
       </c>
       <c r="B265" t="s">
@@ -6065,7 +6075,7 @@
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="4">
+      <c r="A266">
         <v>7502009744013</v>
       </c>
       <c r="B266" t="s">
@@ -6076,7 +6086,7 @@
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267" s="4">
+      <c r="A267">
         <v>7502209290860</v>
       </c>
       <c r="B267" t="s">
@@ -6087,7 +6097,7 @@
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" s="4">
+      <c r="A268">
         <v>7502213144012</v>
       </c>
       <c r="B268" t="s">
@@ -6098,7 +6108,7 @@
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="4">
+      <c r="A269">
         <v>7502216930476</v>
       </c>
       <c r="B269" t="s">
@@ -6109,7 +6119,7 @@
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="4">
+      <c r="A270">
         <v>7502216930551</v>
       </c>
       <c r="B270" t="s">
@@ -6120,7 +6130,7 @@
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="4">
+      <c r="A271">
         <v>7502216930568</v>
       </c>
       <c r="B271" t="s">
@@ -6131,7 +6141,7 @@
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="4">
+      <c r="A272">
         <v>7502216935228</v>
       </c>
       <c r="B272" t="s">
@@ -6142,7 +6152,7 @@
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" s="4">
+      <c r="A273">
         <v>7502216935235</v>
       </c>
       <c r="B273" t="s">
@@ -6153,7 +6163,7 @@
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" s="4">
+      <c r="A274">
         <v>7502216936195</v>
       </c>
       <c r="B274" t="s">
@@ -6164,7 +6174,7 @@
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" s="4">
+      <c r="A275">
         <v>7502235760115</v>
       </c>
       <c r="B275" t="s">
@@ -6175,7 +6185,7 @@
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A276" s="4">
+      <c r="A276">
         <v>7502235760139</v>
       </c>
       <c r="B276" t="s">
@@ -6186,7 +6196,7 @@
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" s="4">
+      <c r="A277">
         <v>7502241941331</v>
       </c>
       <c r="B277" t="s">
@@ -6197,7 +6207,7 @@
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" s="4">
+      <c r="A278">
         <v>7502241941928</v>
       </c>
       <c r="B278" t="s">
@@ -6208,7 +6218,7 @@
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279" s="4">
+      <c r="A279">
         <v>7503003746157</v>
       </c>
       <c r="B279" t="s">
@@ -6219,7 +6229,7 @@
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" s="4">
+      <c r="A280">
         <v>7503003746478</v>
       </c>
       <c r="B280" t="s">
@@ -6230,7 +6240,7 @@
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="4">
+      <c r="A281">
         <v>7503006916472</v>
       </c>
       <c r="B281" t="s">
@@ -6241,7 +6251,7 @@
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="4">
+      <c r="A282">
         <v>7503007704566</v>
       </c>
       <c r="B282" t="s">
@@ -6252,7 +6262,7 @@
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" s="4">
+      <c r="A283">
         <v>7503007704634</v>
       </c>
       <c r="B283" t="s">
@@ -6263,7 +6273,7 @@
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A284" s="4">
+      <c r="A284">
         <v>7503007704658</v>
       </c>
       <c r="B284" t="s">
@@ -6274,7 +6284,7 @@
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A285" s="4">
+      <c r="A285">
         <v>7503007822659</v>
       </c>
       <c r="B285" t="s">
@@ -6285,7 +6295,7 @@
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A286" s="4">
+      <c r="A286">
         <v>7503007822895</v>
       </c>
       <c r="B286" t="s">
@@ -6296,7 +6306,7 @@
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="4">
+      <c r="A287">
         <v>7506317100455</v>
       </c>
       <c r="B287" t="s">
@@ -6307,7 +6317,7 @@
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="4">
+      <c r="A288">
         <v>7703331157506</v>
       </c>
       <c r="B288" t="s">
@@ -6318,7 +6328,7 @@
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A289" s="4">
+      <c r="A289">
         <v>7730979093019</v>
       </c>
       <c r="B289" t="s">
@@ -6329,7 +6339,7 @@
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A290" s="4">
+      <c r="A290">
         <v>7730979093026</v>
       </c>
       <c r="B290" t="s">
@@ -6340,7 +6350,7 @@
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291" s="4">
+      <c r="A291">
         <v>7730979094092</v>
       </c>
       <c r="B291" t="s">
@@ -6351,7 +6361,7 @@
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292" s="4">
+      <c r="A292">
         <v>7730979097192</v>
       </c>
       <c r="B292" t="s">
@@ -6362,7 +6372,7 @@
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" s="4">
+      <c r="A293">
         <v>7841141002712</v>
       </c>
       <c r="B293" t="s">
@@ -6373,7 +6383,7 @@
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" s="4">
+      <c r="A294">
         <v>7841141003900</v>
       </c>
       <c r="B294" t="s">
@@ -6384,7 +6394,7 @@
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A295" s="4">
+      <c r="A295">
         <v>7841141004303</v>
       </c>
       <c r="B295" t="s">
@@ -6395,7 +6405,7 @@
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A296" s="4">
+      <c r="A296">
         <v>7891317019525</v>
       </c>
       <c r="B296" t="s">
@@ -6406,7 +6416,7 @@
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297" s="4">
+      <c r="A297">
         <v>7891317019587</v>
       </c>
       <c r="B297" t="s">
@@ -6417,7 +6427,7 @@
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" s="4">
+      <c r="A298">
         <v>7891317019617</v>
       </c>
       <c r="B298" t="s">
@@ -6428,7 +6438,7 @@
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A299" s="4">
+      <c r="A299">
         <v>7896006201816</v>
       </c>
       <c r="B299" t="s">
@@ -6439,7 +6449,7 @@
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" s="4">
+      <c r="A300">
         <v>7896116865663</v>
       </c>
       <c r="B300" t="s">
@@ -6450,7 +6460,7 @@
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A301" s="4">
+      <c r="A301">
         <v>8027950210473</v>
       </c>
       <c r="B301" t="s">
@@ -6461,7 +6471,7 @@
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A302" s="4">
+      <c r="A302">
         <v>8027950210527</v>
       </c>
       <c r="B302" t="s">
@@ -6472,7 +6482,7 @@
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A303" s="4">
+      <c r="A303">
         <v>8903855059976</v>
       </c>
       <c r="B303" t="s">
@@ -6483,7 +6493,7 @@
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" s="4">
+      <c r="A304">
         <v>8903855060002</v>
       </c>
       <c r="B304" t="s">
@@ -12321,13 +12331,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>341</v>
       </c>
@@ -12349,8 +12361,11 @@
       <c r="G1" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12366,8 +12381,11 @@
       <c r="G2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12383,8 +12401,11 @@
       <c r="G3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12400,8 +12421,11 @@
       <c r="G4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12417,8 +12441,11 @@
       <c r="G5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12434,8 +12461,11 @@
       <c r="G6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12451,8 +12481,11 @@
       <c r="G7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12468,8 +12501,11 @@
       <c r="G8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12485,8 +12521,11 @@
       <c r="G9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12502,8 +12541,11 @@
       <c r="G10">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12519,8 +12561,11 @@
       <c r="G11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12536,8 +12581,11 @@
       <c r="G12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -12553,8 +12601,11 @@
       <c r="G13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12570,8 +12621,11 @@
       <c r="G14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -12587,8 +12641,11 @@
       <c r="G15">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -12604,8 +12661,11 @@
       <c r="G16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12621,8 +12681,11 @@
       <c r="G17">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12638,8 +12701,11 @@
       <c r="G18">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -12655,8 +12721,11 @@
       <c r="G19">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -12672,8 +12741,11 @@
       <c r="G20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12689,8 +12761,11 @@
       <c r="G21">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -12706,8 +12781,11 @@
       <c r="G22">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -12723,8 +12801,11 @@
       <c r="G23">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -12740,8 +12821,11 @@
       <c r="G24">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -12757,8 +12841,11 @@
       <c r="G25">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -12774,8 +12861,11 @@
       <c r="G26">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -12791,8 +12881,11 @@
       <c r="G27">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -12808,8 +12901,11 @@
       <c r="G28">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -12825,8 +12921,11 @@
       <c r="G29">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -12842,8 +12941,11 @@
       <c r="G30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -12859,8 +12961,11 @@
       <c r="G31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -12876,8 +12981,11 @@
       <c r="G32">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -12893,8 +13001,11 @@
       <c r="G33">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -12910,8 +13021,11 @@
       <c r="G34">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -12927,8 +13041,11 @@
       <c r="G35">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -12944,8 +13061,11 @@
       <c r="G36">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -12961,8 +13081,11 @@
       <c r="G37">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -12978,8 +13101,11 @@
       <c r="G38">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -12995,8 +13121,11 @@
       <c r="G39">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -13012,8 +13141,11 @@
       <c r="G40">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -13029,8 +13161,11 @@
       <c r="G41">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -13046,8 +13181,11 @@
       <c r="G42">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -13063,8 +13201,11 @@
       <c r="G43">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -13080,8 +13221,11 @@
       <c r="G44">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -13097,8 +13241,11 @@
       <c r="G45">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -13114,8 +13261,11 @@
       <c r="G46">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -13131,8 +13281,11 @@
       <c r="G47">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -13148,8 +13301,11 @@
       <c r="G48">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -13165,8 +13321,11 @@
       <c r="G49">
         <v>30</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -13182,8 +13341,11 @@
       <c r="G50">
         <v>30</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -13198,6 +13360,9 @@
       </c>
       <c r="G51">
         <v>10</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solo falta comprobar con datos reales funcionalidad
</commit_message>
<xml_diff>
--- a/data/dummy_data.xlsx
+++ b/data/dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\PROJECTS\farmacia_alertas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CF8482-1B6E-45BB-91E7-A5E01E7B235B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998D2729-9709-4609-8DEA-5DBB33B2DAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2569,7 +2569,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -12333,8 +12333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12379,7 +12379,7 @@
         <v>45835</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -12399,7 +12399,7 @@
         <v>45829</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -12419,7 +12419,7 @@
         <v>45822</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -12439,7 +12439,7 @@
         <v>45815</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -12459,7 +12459,7 @@
         <v>45829</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -12479,7 +12479,7 @@
         <v>45835</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -12499,7 +12499,7 @@
         <v>45835</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -12519,7 +12519,7 @@
         <v>45827</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -12539,7 +12539,7 @@
         <v>45818</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>4</v>
@@ -12559,7 +12559,7 @@
         <v>45831</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>5</v>
@@ -12579,7 +12579,7 @@
         <v>45826</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -12599,7 +12599,7 @@
         <v>45836</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -12619,7 +12619,7 @@
         <v>45826</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -12639,7 +12639,7 @@
         <v>45824</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -12659,7 +12659,7 @@
         <v>45814</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>4</v>
@@ -12679,7 +12679,7 @@
         <v>45835</v>
       </c>
       <c r="G17">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -12699,7 +12699,7 @@
         <v>45810</v>
       </c>
       <c r="G18">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -12719,7 +12719,7 @@
         <v>45820</v>
       </c>
       <c r="G19">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -12739,7 +12739,7 @@
         <v>45820</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -12759,7 +12759,7 @@
         <v>45836</v>
       </c>
       <c r="G21">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -12779,7 +12779,7 @@
         <v>45812</v>
       </c>
       <c r="G22">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -12799,7 +12799,7 @@
         <v>45814</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <v>3</v>
@@ -12819,7 +12819,7 @@
         <v>45811</v>
       </c>
       <c r="G24">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H24">
         <v>4</v>
@@ -12839,7 +12839,7 @@
         <v>45820</v>
       </c>
       <c r="G25">
-        <v>30</v>
+        <v>325</v>
       </c>
       <c r="H25">
         <v>5</v>
@@ -12859,7 +12859,7 @@
         <v>45817</v>
       </c>
       <c r="G26">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -12879,7 +12879,7 @@
         <v>45832</v>
       </c>
       <c r="G27">
-        <v>30</v>
+        <v>412</v>
       </c>
       <c r="H27">
         <v>2</v>
@@ -12899,7 +12899,7 @@
         <v>45818</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <v>3</v>
@@ -12919,7 +12919,7 @@
         <v>45829</v>
       </c>
       <c r="G29">
-        <v>30</v>
+        <v>321</v>
       </c>
       <c r="H29">
         <v>4</v>
@@ -12939,7 +12939,7 @@
         <v>45811</v>
       </c>
       <c r="G30">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -12959,7 +12959,7 @@
         <v>45836</v>
       </c>
       <c r="G31">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -12979,7 +12979,7 @@
         <v>45819</v>
       </c>
       <c r="G32">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -12999,7 +12999,7 @@
         <v>45812</v>
       </c>
       <c r="G33">
-        <v>30</v>
+        <v>1312312</v>
       </c>
       <c r="H33">
         <v>3</v>
@@ -13019,7 +13019,7 @@
         <v>45826</v>
       </c>
       <c r="G34">
-        <v>30</v>
+        <v>321</v>
       </c>
       <c r="H34">
         <v>4</v>
@@ -13039,7 +13039,7 @@
         <v>45836</v>
       </c>
       <c r="G35">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H35">
         <v>5</v>
@@ -13059,7 +13059,7 @@
         <v>45834</v>
       </c>
       <c r="G36">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -13079,7 +13079,7 @@
         <v>45833</v>
       </c>
       <c r="G37">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -13099,7 +13099,7 @@
         <v>45818</v>
       </c>
       <c r="G38">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -13119,7 +13119,7 @@
         <v>45826</v>
       </c>
       <c r="G39">
-        <v>30</v>
+        <v>12312</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -13139,7 +13139,7 @@
         <v>45833</v>
       </c>
       <c r="G40">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H40">
         <v>5</v>
@@ -13159,7 +13159,7 @@
         <v>45834</v>
       </c>
       <c r="G41">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -13179,7 +13179,7 @@
         <v>45811</v>
       </c>
       <c r="G42">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -13219,7 +13219,7 @@
         <v>45814</v>
       </c>
       <c r="G44">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -13239,7 +13239,7 @@
         <v>45836</v>
       </c>
       <c r="G45">
-        <v>30</v>
+        <v>312</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -13259,7 +13259,7 @@
         <v>45837</v>
       </c>
       <c r="G46">
-        <v>23</v>
+        <v>312</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -13279,7 +13279,7 @@
         <v>45821</v>
       </c>
       <c r="G47">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -13299,7 +13299,7 @@
         <v>45827</v>
       </c>
       <c r="G48">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="H48">
         <v>3</v>
@@ -13319,7 +13319,7 @@
         <v>45831</v>
       </c>
       <c r="G49">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H49">
         <v>4</v>
@@ -13339,7 +13339,7 @@
         <v>45829</v>
       </c>
       <c r="G50">
-        <v>30</v>
+        <v>13221</v>
       </c>
       <c r="H50">
         <v>5</v>
@@ -13359,7 +13359,7 @@
         <v>45822</v>
       </c>
       <c r="G51">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H51">
         <v>0</v>

</xml_diff>